<commit_message>
Subida con recorridos de r
Todas las cordenadas hechas y los recorridos de las ciudades peta cuando
vamos a canarias el resto no.
</commit_message>
<xml_diff>
--- a/Jon/CiudadesEspaña.xlsx
+++ b/Jon/CiudadesEspaña.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Vitoria</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Badajoz</t>
   </si>
   <si>
-    <t>Palma</t>
-  </si>
-  <si>
     <t>Caceres</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>Ciudades</t>
   </si>
   <si>
-    <t>barcelona</t>
-  </si>
-  <si>
     <t>burgos</t>
   </si>
   <si>
@@ -188,9 +182,6 @@
     <t>-0.4906855</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>-0.0513246</t>
   </si>
   <si>
@@ -206,14 +197,20 @@
     <t>lat</t>
   </si>
   <si>
-    <t>Ion</t>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>Palma de mallorca</t>
+  </si>
+  <si>
+    <t>lon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,13 +233,6 @@
       <b/>
       <sz val="8"/>
       <color rgb="FF555555"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="8"/>
-      <color rgb="FFB0B0B0"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -300,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -317,12 +307,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -335,6 +319,7 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53:C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,587 +646,588 @@
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>42859134</v>
+        <v>-26818614</v>
       </c>
       <c r="C2" s="1">
-        <v>-26818614</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4285913</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
-        <v>38994349</v>
-      </c>
-      <c r="C3" s="3">
-        <v>-18585424</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="9">
+        <v>-1858542</v>
+      </c>
+      <c r="C3" s="9">
+        <v>3899435</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>38345996</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3834600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>36834047</v>
+        <v>-24637136</v>
       </c>
       <c r="C5" s="3">
-        <v>-24637136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>3683405</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
-        <v>40656685</v>
-      </c>
-      <c r="C6" s="1">
-        <v>-46812086</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9">
+        <v>-4681209</v>
+      </c>
+      <c r="C6" s="9">
+        <v>4065669</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3">
+        <v>-69706535</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3887945</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="1">
+        <v>26501603</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3956960</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="9">
+        <v>2173404</v>
+      </c>
+      <c r="C9" s="9">
+        <v>4138506</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-36969060</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4234399</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="B11" s="3">
+        <v>-63724247</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3947528</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-62885962</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3652706</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3998636</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="9">
+        <v>-3927378</v>
+      </c>
+      <c r="C14" s="9">
+        <v>3898483</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3">
+        <v>-47793835</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3788818</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="3">
-        <v>41385064</v>
-      </c>
-      <c r="C9" s="3">
-        <v>21734035</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="1">
-        <v>42343992</v>
-      </c>
-      <c r="C10" s="1">
-        <v>-36969060</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3">
-        <v>39475276</v>
-      </c>
-      <c r="C11" s="3">
-        <v>-63724247</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3">
-        <v>39986356</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1">
-        <v>38984829</v>
-      </c>
-      <c r="C14" s="1">
-        <v>-39273778</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="3">
-        <v>37888175</v>
-      </c>
-      <c r="C15" s="3">
-        <v>-47793835</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="11">
-        <v>-841154</v>
-      </c>
-      <c r="C16" s="11">
+      <c r="B16" s="1">
+        <v>-84115401</v>
+      </c>
+      <c r="C16" s="1">
         <v>4336234</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="3">
+        <v>33</v>
+      </c>
+      <c r="B17" s="9">
+        <v>-790059</v>
+      </c>
+      <c r="C17" s="9">
         <v>-2900129</v>
-      </c>
-      <c r="C17" s="3">
-        <v>-790058965</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="1">
-        <v>41979400</v>
+        <v>28214264</v>
       </c>
       <c r="C18" s="1">
-        <v>28214264</v>
+        <v>4197940</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="3">
-        <v>41980225</v>
-      </c>
-      <c r="C19" s="3">
-        <v>-892201577</v>
+        <v>34</v>
+      </c>
+      <c r="B19" s="9">
+        <v>-8922016</v>
+      </c>
+      <c r="C19" s="9">
+        <v>4198023</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="11">
-        <v>-1033496</v>
-      </c>
-      <c r="C20" s="11">
-        <v>206597</v>
+        <v>35</v>
+      </c>
+      <c r="B20" s="1">
+        <v>-1033496092</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2065970</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" s="3">
-        <v>40726646</v>
+        <v>-739798858</v>
       </c>
       <c r="C21" s="3">
-        <v>-739798858</v>
+        <v>4072665</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="11">
-        <v>-6944722</v>
-      </c>
-      <c r="C22" s="11">
+        <v>37</v>
+      </c>
+      <c r="B22" s="1">
+        <v>-69447224</v>
+      </c>
+      <c r="C22" s="1">
         <v>3726142</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="3">
-        <v>42131845</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>56</v>
+        <v>36</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="3">
+        <v>4213184</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="1">
-        <v>37779594</v>
-      </c>
-      <c r="C24" s="1">
-        <v>-37849057</v>
+        <v>13</v>
+      </c>
+      <c r="B24" s="9">
+        <v>-3784906</v>
+      </c>
+      <c r="C24" s="9">
+        <v>3777959</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" s="3">
-        <v>30490618</v>
+        <v>-55670959</v>
       </c>
       <c r="C25" s="3">
-        <v>-841857115</v>
+        <v>4259873</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="1">
-        <v>41617590</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>57</v>
+        <v>38</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="1">
+        <v>4161759</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B27" s="3">
-        <v>42462719</v>
+        <v>-24449852</v>
       </c>
       <c r="C27" s="3">
-        <v>-24449852</v>
+        <v>4246272</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>54</v>
+        <v>39</v>
+      </c>
+      <c r="B28" s="1">
+        <v>-75567582</v>
+      </c>
+      <c r="C28" s="1">
+        <v>4300974</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>54</v>
+        <v>41</v>
+      </c>
+      <c r="B29" s="3">
+        <v>-37037902</v>
+      </c>
+      <c r="C29" s="3">
+        <v>4041678</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1">
-        <v>36721274</v>
+        <v>-44213988</v>
       </c>
       <c r="C30" s="1">
-        <v>-44213988</v>
+        <v>3672127</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" s="3">
-        <v>37992240</v>
+        <v>-11306544</v>
       </c>
       <c r="C31" s="3">
-        <v>-11306544</v>
+        <v>3799224</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B32" s="1">
-        <v>42812526</v>
+        <v>-16457745</v>
       </c>
       <c r="C32" s="1">
-        <v>-16457745</v>
+        <v>4281253</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B33" s="3">
-        <v>42335789</v>
+        <v>-78638810</v>
       </c>
       <c r="C33" s="3">
-        <v>-78638810</v>
+        <v>4233579</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="1">
-        <v>28669997</v>
+        <v>-812081203</v>
       </c>
       <c r="C34" s="1">
-        <v>-812081203</v>
+        <v>2867000</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" s="3">
-        <v>30026159</v>
+        <v>-813856257</v>
       </c>
       <c r="C35" s="3">
-        <v>-813856257</v>
+        <v>3002616</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="B36" s="1">
+        <v>-154362574</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2812355</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B37" s="3">
-        <v>42429885</v>
+        <v>-86446202</v>
       </c>
       <c r="C37" s="3">
-        <v>-86446202</v>
+        <v>4242988</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>54</v>
+        <v>19</v>
+      </c>
+      <c r="B38" s="1">
+        <v>-56635397</v>
+      </c>
+      <c r="C38" s="1">
+        <v>4097010</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="3">
-        <v>28463630</v>
-      </c>
-      <c r="C39" s="3">
-        <v>-162518467</v>
+        <v>20</v>
+      </c>
+      <c r="B39" s="9">
+        <v>-1625185</v>
+      </c>
+      <c r="C39" s="9">
+        <v>2846363</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B40" s="1">
-        <v>32807752</v>
+        <v>-968681303</v>
       </c>
       <c r="C40" s="1">
-        <v>-968681303</v>
+        <v>3280775</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B41" s="3">
-        <v>40942903</v>
+        <v>-41088069</v>
       </c>
       <c r="C41" s="3">
-        <v>-41088069</v>
+        <v>4094290</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B42" s="1">
-        <v>37389092</v>
+        <v>-59844589</v>
       </c>
       <c r="C42" s="1">
-        <v>-59844589</v>
+        <v>3738909</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B43" s="3">
-        <v>41766597</v>
+        <v>-24790306</v>
       </c>
       <c r="C43" s="3">
-        <v>-24790306</v>
+        <v>4176660</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B44" s="1">
-        <v>41118883</v>
+        <v>12444909</v>
       </c>
       <c r="C44" s="1">
-        <v>12444909</v>
+        <v>4111888</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45" s="3">
-        <v>40345688</v>
+        <v>-11064345</v>
       </c>
       <c r="C45" s="3">
-        <v>-11064345</v>
+        <v>4034569</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B46" s="1">
-        <v>41663938</v>
+        <v>-835552120</v>
       </c>
       <c r="C46" s="1">
-        <v>-835552120</v>
+        <v>4166394</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B47" s="3">
-        <v>28521294</v>
+        <v>-814657554</v>
       </c>
       <c r="C47" s="3">
-        <v>-814657554</v>
+        <v>2852129</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>54</v>
+        <v>25</v>
+      </c>
+      <c r="B48" s="1">
+        <v>-47245321</v>
+      </c>
+      <c r="C48" s="1">
+        <v>4165225</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>54</v>
+        <v>26</v>
+      </c>
+      <c r="B49" s="3">
+        <v>-29349852</v>
+      </c>
+      <c r="C49" s="3">
+        <v>4326301</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="B50" s="1">
+        <v>-57467879</v>
+      </c>
+      <c r="C50" s="1">
+        <v>4150347</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B51" s="3">
-        <v>41648823</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>58</v>
+        <v>27</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="3">
+        <v>4164882</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B52" s="1">
-        <v>35889387</v>
+        <v>-53213455</v>
       </c>
       <c r="C52" s="1">
-        <v>-53213455</v>
+        <v>3588939</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B53" s="3">
-        <v>35292277</v>
-      </c>
-      <c r="C53" s="3">
-        <v>-29380973</v>
+        <v>29</v>
+      </c>
+      <c r="B53" s="9">
+        <v>-2938097</v>
+      </c>
+      <c r="C53" s="9">
+        <v>3529228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglado todas las distancias y los tiempo
Falta eliminar la columna 1 y la fila 1
</commit_message>
<xml_diff>
--- a/Jon/CiudadesEspaña.xlsx
+++ b/Jon/CiudadesEspaña.xlsx
@@ -68,9 +68,6 @@
     <t>Jaen</t>
   </si>
   <si>
-    <t>Leon</t>
-  </si>
-  <si>
     <t>Murcia</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>Salamanca</t>
   </si>
   <si>
-    <t>Santa Cruz de Tenerife</t>
-  </si>
-  <si>
     <t>Sevilla</t>
   </si>
   <si>
@@ -125,15 +119,6 @@
     <t>coruna</t>
   </si>
   <si>
-    <t>cuenca</t>
-  </si>
-  <si>
-    <t>chana</t>
-  </si>
-  <si>
-    <t>guadalajara</t>
-  </si>
-  <si>
     <t>huesca</t>
   </si>
   <si>
@@ -164,9 +149,6 @@
     <t>pontevedra</t>
   </si>
   <si>
-    <t>santander</t>
-  </si>
-  <si>
     <t>segovia</t>
   </si>
   <si>
@@ -197,20 +179,38 @@
     <t>lat</t>
   </si>
   <si>
-    <t>Barcelona</t>
-  </si>
-  <si>
     <t>Palma de mallorca</t>
   </si>
   <si>
     <t>lon</t>
+  </si>
+  <si>
+    <t>Tenerife</t>
+  </si>
+  <si>
+    <t>Granada</t>
+  </si>
+  <si>
+    <t>Centro Comercial Ferial Plaza, Guadalajara</t>
+  </si>
+  <si>
+    <t>Catedral de Leon</t>
+  </si>
+  <si>
+    <t>Parque De Santa Ana, Cuenca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Passeig de Colom, Barcelona </t>
+  </si>
+  <si>
+    <t>Catedral de Santander</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +236,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -258,13 +265,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,7 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -335,16 +342,26 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -661,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,13 +691,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -710,7 +727,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1">
         <v>3834600</v>
@@ -751,7 +768,7 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1">
         <v>26501603</v>
@@ -761,19 +778,19 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="11">
+      <c r="A9" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="15">
         <v>2173404</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="15">
         <v>4138506</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1">
         <v>-36969060</v>
@@ -809,7 +826,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C13" s="3">
         <v>3998636</v>
@@ -838,57 +855,57 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="14">
+      <c r="A16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="11">
         <v>-84115401</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="11">
         <v>4336234</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="11">
+      <c r="A17" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="15">
         <v>-790059</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="15">
         <v>-2900129</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="13">
         <v>28214264</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="13">
         <v>4197940</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="11">
+      <c r="A19" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="15">
         <v>-8922016</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="15">
         <v>4198023</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="12">
+      <c r="A20" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="13">
         <v>-1033496092</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="13">
         <v>2065970</v>
       </c>
     </row>
@@ -905,7 +922,7 @@
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1">
         <v>-69447224</v>
@@ -916,10 +933,10 @@
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C23" s="3">
         <v>4213184</v>
@@ -937,22 +954,22 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="12">
+      <c r="A25" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="13">
         <v>-55670959</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="13">
         <v>4259873</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C26" s="1">
         <v>4161759</v>
@@ -960,7 +977,7 @@
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B27" s="3">
         <v>-24449852</v>
@@ -971,7 +988,7 @@
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1">
         <v>-75567582</v>
@@ -982,7 +999,7 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B29" s="3">
         <v>-37037902</v>
@@ -993,7 +1010,7 @@
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1">
         <v>-44213988</v>
@@ -1004,7 +1021,7 @@
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" s="3">
         <v>-11306544</v>
@@ -1015,7 +1032,7 @@
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B32" s="1">
         <v>-16457745</v>
@@ -1026,7 +1043,7 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B33" s="3">
         <v>-78638810</v>
@@ -1037,7 +1054,7 @@
     </row>
     <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B34" s="1">
         <v>-812081203</v>
@@ -1048,7 +1065,7 @@
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" s="3">
         <v>-813856257</v>
@@ -1059,7 +1076,7 @@
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" s="1">
         <v>-154362574</v>
@@ -1070,7 +1087,7 @@
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B37" s="3">
         <v>-86446202</v>
@@ -1081,7 +1098,7 @@
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38" s="1">
         <v>-56635397</v>
@@ -1090,168 +1107,168 @@
         <v>4097010</v>
       </c>
     </row>
+    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="16">
+        <v>-968681303</v>
+      </c>
+      <c r="C39" s="16">
+        <v>3280775</v>
+      </c>
+    </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="1">
-        <v>-968681303</v>
-      </c>
-      <c r="C40" s="1">
-        <v>3280775</v>
+      <c r="A40" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="3">
+        <v>-41088069</v>
+      </c>
+      <c r="C40" s="3">
+        <v>4094290</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41" s="3">
-        <v>-41088069</v>
-      </c>
-      <c r="C41" s="3">
-        <v>4094290</v>
+      <c r="A41" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="13">
+        <v>-59844589</v>
+      </c>
+      <c r="C41" s="13">
+        <v>3738909</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="13">
+        <v>-24790306</v>
+      </c>
+      <c r="C42" s="13">
+        <v>4176660</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="13">
+        <v>12444909</v>
+      </c>
+      <c r="C43" s="13">
+        <v>4111888</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="1">
-        <v>-59844589</v>
-      </c>
-      <c r="C42" s="1">
-        <v>3738909</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="B44" s="13">
+        <v>-11064345</v>
+      </c>
+      <c r="C44" s="13">
+        <v>4034569</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="3">
-        <v>-24790306</v>
-      </c>
-      <c r="C43" s="3">
-        <v>4176660</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="1">
-        <v>12444909</v>
-      </c>
-      <c r="C44" s="1">
-        <v>4111888</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="B45" s="13">
+        <v>-835552120</v>
+      </c>
+      <c r="C45" s="13">
+        <v>4166394</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="13">
+        <v>-814657554</v>
+      </c>
+      <c r="C46" s="13">
+        <v>2852129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="3">
-        <v>-11064345</v>
-      </c>
-      <c r="C45" s="3">
-        <v>4034569</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
+      <c r="B47" s="13">
+        <v>-47245321</v>
+      </c>
+      <c r="C47" s="13">
+        <v>4165225</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B46" s="1">
-        <v>-835552120</v>
-      </c>
-      <c r="C46" s="1">
-        <v>4166394</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="B48" s="13">
+        <v>-29349852</v>
+      </c>
+      <c r="C48" s="13">
+        <v>4326301</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" s="13">
+        <v>-57467879</v>
+      </c>
+      <c r="C49" s="13">
+        <v>4150347</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="3">
-        <v>-814657554</v>
-      </c>
-      <c r="C47" s="3">
-        <v>2852129</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B48" s="1">
-        <v>-47245321</v>
-      </c>
-      <c r="C48" s="1">
-        <v>4165225</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="C50" s="13">
+        <v>4164882</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B49" s="3">
-        <v>-29349852</v>
-      </c>
-      <c r="C49" s="3">
-        <v>4326301</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="1">
-        <v>-57467879</v>
-      </c>
-      <c r="C50" s="1">
-        <v>4150347</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="B51" s="13">
+        <v>-53213455</v>
+      </c>
+      <c r="C51" s="13">
+        <v>3588939</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C51" s="3">
-        <v>4164882</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B52" s="1">
-        <v>-53213455</v>
-      </c>
-      <c r="C52" s="1">
-        <v>3588939</v>
+      <c r="B52" s="15">
+        <v>-2938097</v>
+      </c>
+      <c r="C52" s="15">
+        <v>3529228</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B53" s="9">
-        <v>-2938097</v>
-      </c>
-      <c r="C53" s="9">
-        <v>3529228</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B54" s="11">
+      <c r="A53" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="15">
         <v>-1625185</v>
       </c>
-      <c r="C54" s="11">
+      <c r="C53" s="15">
         <v>2846363</v>
       </c>
     </row>

</xml_diff>